<commit_message>
run modelv5 at all depths
</commit_message>
<xml_diff>
--- a/scripts/Data/00_modelv4error.xlsx
+++ b/scripts/Data/00_modelv4error.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colette/Box Sync/N2O Research/ETNP 2018/Data/isotopomer-soup/scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246C4FA5-7F3A-F242-AD8F-6AA220B7CF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4C2D83-B9D5-4D41-BF8A-102AD0622CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18580" yWindow="-5500" windowWidth="18580" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18580" yWindow="-5500" windowWidth="18580" windowHeight="23060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -567,11 +567,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Run errors for modelv5
</commit_message>
<xml_diff>
--- a/scripts/Data/00_modelv4error.xlsx
+++ b/scripts/Data/00_modelv4error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colette/Box Sync/N2O Research/ETNP 2018/Data/isotopomer-soup/scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4C2D83-B9D5-4D41-BF8A-102AD0622CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4397BB12-F643-5B4B-A16C-83B4C90EC244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18580" yWindow="-5500" windowWidth="18580" windowHeight="23060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:XFD53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add datapath to runscript saveout
</commit_message>
<xml_diff>
--- a/scripts/Data/00_modelv4error.xlsx
+++ b/scripts/Data/00_modelv4error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colette/Box Sync/N2O Research/ETNP 2018/Data/isotopomer-soup/scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4397BB12-F643-5B4B-A16C-83B4C90EC244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C0D486-DF38-9141-900B-8957970E9B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18580" yWindow="-5500" windowWidth="18580" windowHeight="23060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adjust weights in run_errors.py
</commit_message>
<xml_diff>
--- a/scripts/Data/00_modelv4error.xlsx
+++ b/scripts/Data/00_modelv4error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colette/Box Sync/N2O Research/ETNP 2018/Data/isotopomer-soup/scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C0D486-DF38-9141-900B-8957970E9B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F44E81-19E1-FA40-A050-1DB8E32DAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18580" yWindow="-5500" windowWidth="18580" windowHeight="23060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16380" yWindow="500" windowWidth="12400" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>